<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@8675334f1b2db40d1bcb14d8f2742c7a1e5df0fc 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-test-binding.xlsx
+++ b/StructureDefinition-test-binding.xlsx
@@ -483,10 +483,10 @@
 </t>
   </si>
   <si>
-    <t>Kind of referral</t>
-  </si>
-  <si>
-    <t>Identifies the type of referral, constrained to valid HL7 attachment request codes from LOINC.</t>
+    <t>Kind of attachment</t>
+  </si>
+  <si>
+    <t>constrained to valid HL7 attachment request codes from LOINC.</t>
   </si>
   <si>
     <t>Because resource references will only be able to indicate 'Basic', the type of reference will need to be specified in a Profile identified as part of the resource.  Refer to the resource notes section for information on appropriate terminologies for this code.

</xml_diff>